<commit_message>
Papers review for state of art
</commit_message>
<xml_diff>
--- a/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
+++ b/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haachicanoy/Repositories/CSmaster/_semester_1/_introduction_to_research/_workshops_training/Taller 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToBackup\repositories\personal\CSmaster\_semester_1\_introduction_to_research\_workshops_training\Taller 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14840"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14844"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -308,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -328,6 +325,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,21 +611,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="37.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -642,14 +642,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="157" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="156.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>2017</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -659,7 +659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="157" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="168.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2017</v>
       </c>
@@ -676,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="181" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="180.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2017</v>
       </c>
@@ -693,7 +693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="169" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="168.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2017</v>
       </c>
@@ -710,7 +710,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="121" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="120.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>2015</v>
       </c>
@@ -727,7 +727,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="109" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="120.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2014</v>
       </c>
@@ -744,7 +744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="193.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2015</v>
       </c>
@@ -761,7 +761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="186.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="186.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2017</v>
       </c>
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="133" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>2016</v>
       </c>
@@ -795,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="157" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="156.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>2017</v>
       </c>
@@ -812,10 +812,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" ht="43.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="43.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="43.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="43.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Starting final exam of fdb
</commit_message>
<xml_diff>
--- a/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
+++ b/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
@@ -612,8 +612,8 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +666,7 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -683,7 +683,7 @@
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">

</xml_diff>

<commit_message>
State of art almost done
</commit_message>
<xml_diff>
--- a/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
+++ b/_semester_1/_introduction_to_research/_workshops_training/Taller 3/Bibliografia_anotada.xlsx
@@ -66,17 +66,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> @article{Basso:2014,
- author = {Basso, Bruno and Cammarano, Davide and De Vita, Pasquale},
- year = {2004},
- month = {01},
- pages = {36-53},
- title = {Remotely sensed vegetation indices: theory and application for crop management},
- volume = {1},
- booktitle = {Rivista Italiana di Agrometeorologia}
-}</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @article{Sahoo:2015,
  author = {Sahoo, Rabi and Ray, Shibendu and R, Manjunath},
  year = {2015},
@@ -234,6 +223,17 @@
   </si>
   <si>
     <t>Análisis fractal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @article{Basso:2004,
+ author = {Basso, Bruno and Cammarano, Davide and De Vita, Pasquale},
+ year = {2004},
+ month = {01},
+ pages = {36-53},
+ title = {Remotely sensed vegetation indices: theory and application for crop management},
+ volume = {1},
+ booktitle = {Rivista Italiana di Agrometeorologia}
+}</t>
   </si>
 </sst>
 </file>
@@ -305,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -328,6 +328,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,8 +615,8 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -647,16 +650,16 @@
         <v>2017</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="168.6" x14ac:dyDescent="0.3">
@@ -664,16 +667,16 @@
         <v>2017</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="180.6" x14ac:dyDescent="0.3">
@@ -681,16 +684,16 @@
         <v>2017</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="168.6" x14ac:dyDescent="0.3">
@@ -698,16 +701,16 @@
         <v>2017</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="120.6" x14ac:dyDescent="0.3">
@@ -715,16 +718,16 @@
         <v>2015</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="120.6" x14ac:dyDescent="0.3">
@@ -732,16 +735,16 @@
         <v>2014</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -749,10 +752,10 @@
         <v>2015</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>4</v>
@@ -766,10 +769,10 @@
         <v>2017</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -783,10 +786,10 @@
         <v>2016</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
@@ -800,16 +803,16 @@
         <v>2017</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>